<commit_message>
Changes to docs + comments
</commit_message>
<xml_diff>
--- a/EvenementsEnDirect/docs/analyse/Planification TPI Davila 2020.xlsx
+++ b/EvenementsEnDirect/docs/analyse/Planification TPI Davila 2020.xlsx
@@ -303,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -373,6 +373,9 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
@@ -389,9 +392,6 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -415,21 +415,27 @@
     <xf borderId="0" fillId="3" fontId="5" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="21" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="4" fillId="3" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="4" fillId="3" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
@@ -442,14 +448,14 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -778,10 +784,10 @@
       <c r="B4" s="16">
         <v>0.0625</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="13"/>
+      <c r="D4" s="13">
         <v>0.0625</v>
       </c>
-      <c r="D4" s="14"/>
       <c r="E4" s="9"/>
       <c r="F4" s="14"/>
       <c r="G4" s="9"/>
@@ -803,10 +809,10 @@
         <v>0.0625</v>
       </c>
       <c r="C5" s="17"/>
-      <c r="D5" s="13">
+      <c r="D5" s="13"/>
+      <c r="E5" s="7">
         <v>0.0625</v>
       </c>
-      <c r="E5" s="9"/>
       <c r="F5" s="14"/>
       <c r="G5" s="9"/>
       <c r="H5" s="14"/>
@@ -827,9 +833,11 @@
         <v>0.25</v>
       </c>
       <c r="C6" s="19">
-        <v>0.25</v>
-      </c>
-      <c r="D6" s="14"/>
+        <v>0.1875</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.0625</v>
+      </c>
       <c r="E6" s="9"/>
       <c r="F6" s="14"/>
       <c r="G6" s="9"/>
@@ -851,10 +859,10 @@
         <v>0.020833333333333332</v>
       </c>
       <c r="C7" s="17"/>
-      <c r="D7" s="13">
+      <c r="D7" s="13"/>
+      <c r="E7" s="7">
         <v>0.020833333333333332</v>
       </c>
-      <c r="E7" s="9"/>
       <c r="F7" s="14"/>
       <c r="G7" s="9"/>
       <c r="H7" s="14"/>
@@ -940,11 +948,11 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="23">
+      <c r="G11" s="23">
         <v>0.020833333333333332</v>
       </c>
-      <c r="I11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
       <c r="J11" s="14"/>
       <c r="K11" s="8"/>
       <c r="L11" s="15"/>
@@ -957,18 +965,18 @@
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="25">
         <v>0.020833333333333332</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="13"/>
       <c r="E12" s="7"/>
       <c r="F12" s="14"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="25">
+      <c r="G12" s="23">
         <v>0.020833333333333332</v>
       </c>
-      <c r="I12" s="25"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
       <c r="J12" s="14"/>
       <c r="K12" s="8"/>
       <c r="L12" s="15"/>
@@ -981,7 +989,7 @@
       <c r="A13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="25">
         <v>0.041666666666666664</v>
       </c>
       <c r="C13" s="8"/>
@@ -989,10 +997,10 @@
       <c r="E13" s="7"/>
       <c r="F13" s="14"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="26">
+      <c r="H13" s="27">
         <v>0.041666666666666664</v>
       </c>
-      <c r="I13" s="25"/>
+      <c r="I13" s="26"/>
       <c r="J13" s="14"/>
       <c r="K13" s="8"/>
       <c r="L13" s="15"/>
@@ -1005,17 +1013,17 @@
       <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="25">
         <v>0.041666666666666664</v>
       </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="23"/>
       <c r="F14" s="14"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="29">
+      <c r="G14" s="23">
         <v>0.041666666666666664</v>
       </c>
+      <c r="H14" s="29"/>
       <c r="I14" s="29"/>
       <c r="J14" s="14"/>
       <c r="K14" s="8"/>
@@ -1029,7 +1037,7 @@
       <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="25">
         <v>0.041666666666666664</v>
       </c>
       <c r="C15" s="8"/>
@@ -1038,10 +1046,10 @@
       <c r="F15" s="14"/>
       <c r="G15" s="8"/>
       <c r="H15" s="30"/>
-      <c r="I15" s="26">
+      <c r="I15" s="27"/>
+      <c r="J15" s="13">
         <v>0.041666666666666664</v>
       </c>
-      <c r="J15" s="14"/>
       <c r="K15" s="8"/>
       <c r="L15" s="15"/>
       <c r="M15" s="11">
@@ -1062,12 +1070,12 @@
       <c r="F16" s="33"/>
       <c r="G16" s="35"/>
       <c r="H16" s="36"/>
-      <c r="I16" s="26">
+      <c r="I16" s="27">
         <v>0.041666666666666664</v>
       </c>
-      <c r="J16" s="33"/>
+      <c r="J16" s="37"/>
       <c r="K16" s="32"/>
-      <c r="L16" s="37"/>
+      <c r="L16" s="38"/>
       <c r="M16" s="11">
         <f t="shared" si="1"/>
         <v>0.04166666667</v>
@@ -1077,18 +1085,18 @@
       <c r="A17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="25">
         <v>0.041666666666666664</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="14"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="26">
+      <c r="F17" s="28"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="40">
         <v>0.041666666666666664</v>
       </c>
+      <c r="I17" s="27"/>
       <c r="J17" s="14"/>
       <c r="K17" s="8"/>
       <c r="L17" s="15"/>
@@ -1101,19 +1109,19 @@
       <c r="A18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="25">
         <v>0.041666666666666664</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="14"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="27"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="28"/>
       <c r="G18" s="17"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29">
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="13">
         <v>0.041666666666666664</v>
       </c>
-      <c r="J18" s="14"/>
       <c r="K18" s="8"/>
       <c r="L18" s="15"/>
       <c r="M18" s="11">
@@ -1123,13 +1131,13 @@
     </row>
     <row r="19">
       <c r="A19" s="5"/>
-      <c r="B19" s="24"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="8"/>
       <c r="D19" s="14"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="27"/>
+      <c r="F19" s="28"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="27"/>
+      <c r="H19" s="28"/>
       <c r="I19" s="8"/>
       <c r="J19" s="14"/>
       <c r="K19" s="8"/>
@@ -1145,7 +1153,7 @@
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="27"/>
+      <c r="D20" s="28"/>
       <c r="E20" s="9"/>
       <c r="F20" s="14"/>
       <c r="G20" s="9"/>
@@ -1167,8 +1175,8 @@
         <v>0.08333333333333333</v>
       </c>
       <c r="C21" s="9"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="23">
+      <c r="D21" s="28"/>
+      <c r="E21" s="24">
         <v>0.08333333333333333</v>
       </c>
       <c r="F21" s="13"/>
@@ -1192,16 +1200,16 @@
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="14"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="7">
+      <c r="E22" s="13"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7">
         <v>0.020833333333333332</v>
       </c>
-      <c r="G22" s="7"/>
       <c r="H22" s="14"/>
       <c r="I22" s="17"/>
       <c r="J22" s="14"/>
       <c r="K22" s="9"/>
-      <c r="L22" s="39"/>
+      <c r="L22" s="41"/>
       <c r="M22" s="11">
         <f t="shared" si="1"/>
         <v>0.02083333333</v>
@@ -1215,17 +1223,17 @@
         <v>0.08333333333333333</v>
       </c>
       <c r="C23" s="9"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="23">
+      <c r="D23" s="28"/>
+      <c r="E23" s="24">
         <v>0.08333333333333333</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="27"/>
+      <c r="H23" s="28"/>
       <c r="I23" s="17"/>
       <c r="J23" s="14"/>
       <c r="K23" s="9"/>
-      <c r="L23" s="39"/>
+      <c r="L23" s="41"/>
       <c r="M23" s="11">
         <f t="shared" si="1"/>
         <v>0.08333333333</v>
@@ -1235,23 +1243,23 @@
       <c r="A24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="24">
+      <c r="B24" s="25">
         <v>0.125</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="14"/>
-      <c r="E24" s="29">
-        <v>0.08333333333333333</v>
-      </c>
-      <c r="F24" s="26">
+      <c r="E24" s="19">
         <v>0.041666666666666664</v>
+      </c>
+      <c r="F24" s="42">
+        <v>0.08333333333333333</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="14"/>
       <c r="I24" s="9"/>
       <c r="J24" s="14"/>
       <c r="K24" s="9"/>
-      <c r="L24" s="39"/>
+      <c r="L24" s="41"/>
       <c r="M24" s="11">
         <f t="shared" si="1"/>
         <v>0.125</v>
@@ -1261,7 +1269,7 @@
       <c r="A25" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="40"/>
+      <c r="B25" s="43"/>
       <c r="C25" s="9"/>
       <c r="D25" s="14"/>
       <c r="E25" s="9"/>
@@ -1271,7 +1279,7 @@
       <c r="I25" s="9"/>
       <c r="J25" s="14"/>
       <c r="K25" s="9"/>
-      <c r="L25" s="39"/>
+      <c r="L25" s="41"/>
       <c r="M25" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1281,7 +1289,7 @@
       <c r="A26" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="24">
+      <c r="B26" s="25">
         <v>0.08333333333333333</v>
       </c>
       <c r="C26" s="9"/>
@@ -1295,7 +1303,7 @@
       <c r="I26" s="9"/>
       <c r="J26" s="14"/>
       <c r="K26" s="9"/>
-      <c r="L26" s="39"/>
+      <c r="L26" s="41"/>
       <c r="M26" s="11">
         <f t="shared" si="1"/>
         <v>0.08333333333</v>
@@ -1305,21 +1313,21 @@
       <c r="A27" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="24">
+      <c r="B27" s="25">
         <v>0.08333333333333333</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="14"/>
       <c r="E27" s="9"/>
-      <c r="F27" s="29">
-        <v>0.08333333333333333</v>
-      </c>
-      <c r="G27" s="7"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="14"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="7">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="H27" s="13"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="13"/>
       <c r="K27" s="9"/>
-      <c r="L27" s="39"/>
+      <c r="L27" s="41"/>
       <c r="M27" s="11">
         <f t="shared" si="1"/>
         <v>0.08333333333</v>
@@ -1333,19 +1341,17 @@
         <v>0.08333333333333333</v>
       </c>
       <c r="C28" s="17"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="26">
-        <v>0.041666666666666664</v>
-      </c>
-      <c r="G28" s="41">
-        <v>0.041666666666666664</v>
-      </c>
-      <c r="H28" s="41"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="42"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="27">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="K28" s="28"/>
+      <c r="L28" s="44"/>
       <c r="M28" s="11">
         <f t="shared" si="1"/>
         <v>0.08333333333</v>
@@ -1365,7 +1371,7 @@
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
       <c r="K29" s="17"/>
-      <c r="L29" s="42"/>
+      <c r="L29" s="44"/>
       <c r="M29" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1381,15 +1387,15 @@
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="29">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="F30" s="20">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="G30" s="29"/>
       <c r="H30" s="7"/>
       <c r="I30" s="17"/>
       <c r="J30" s="17"/>
       <c r="K30" s="9"/>
-      <c r="L30" s="42"/>
+      <c r="L30" s="44"/>
       <c r="M30" s="11">
         <f t="shared" si="1"/>
         <v>0.08333333333</v>
@@ -1409,14 +1415,14 @@
       <c r="I31" s="17"/>
       <c r="J31" s="17"/>
       <c r="K31" s="17"/>
-      <c r="L31" s="39"/>
+      <c r="L31" s="41"/>
       <c r="M31" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="45" t="s">
         <v>41</v>
       </c>
       <c r="B32" s="18">
@@ -1426,14 +1432,14 @@
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="29">
-        <v>0.08333333333333333</v>
-      </c>
-      <c r="H32" s="7"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="7">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="17"/>
-      <c r="L32" s="44"/>
+      <c r="L32" s="46"/>
       <c r="M32" s="11">
         <f t="shared" si="1"/>
         <v>0.08333333333</v>
@@ -1443,7 +1449,7 @@
       <c r="A33" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="45"/>
+      <c r="B33" s="47"/>
       <c r="C33" s="35"/>
       <c r="D33" s="33"/>
       <c r="E33" s="35"/>
@@ -1453,7 +1459,7 @@
       <c r="I33" s="35"/>
       <c r="J33" s="33"/>
       <c r="K33" s="35"/>
-      <c r="L33" s="37"/>
+      <c r="L33" s="38"/>
       <c r="M33" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1471,13 +1477,13 @@
       <c r="E34" s="35"/>
       <c r="F34" s="33"/>
       <c r="G34" s="33"/>
-      <c r="H34" s="29">
+      <c r="H34" s="19">
         <v>0.08333333333333333</v>
       </c>
       <c r="I34" s="34"/>
       <c r="J34" s="33"/>
       <c r="K34" s="35"/>
-      <c r="L34" s="37"/>
+      <c r="L34" s="38"/>
       <c r="M34" s="11">
         <f t="shared" si="1"/>
         <v>0.08333333333</v>
@@ -1494,24 +1500,22 @@
       <c r="D35" s="33"/>
       <c r="E35" s="35"/>
       <c r="F35" s="33"/>
-      <c r="G35" s="46">
-        <v>0.041666666666666664</v>
-      </c>
-      <c r="H35" s="29">
-        <v>0.08333333333333333</v>
-      </c>
-      <c r="I35" s="34"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="34">
+        <v>0.125</v>
+      </c>
       <c r="J35" s="33"/>
       <c r="K35" s="35"/>
-      <c r="L35" s="37"/>
+      <c r="L35" s="38"/>
       <c r="M35" s="11">
         <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="47"/>
-      <c r="B36" s="45"/>
+      <c r="A36" s="48"/>
+      <c r="B36" s="47"/>
       <c r="C36" s="35"/>
       <c r="D36" s="33"/>
       <c r="E36" s="35"/>
@@ -1521,7 +1525,7 @@
       <c r="I36" s="35"/>
       <c r="J36" s="33"/>
       <c r="K36" s="35"/>
-      <c r="L36" s="37"/>
+      <c r="L36" s="38"/>
       <c r="M36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1541,7 +1545,7 @@
       <c r="I37" s="17"/>
       <c r="J37" s="17"/>
       <c r="K37" s="17"/>
-      <c r="L37" s="39"/>
+      <c r="L37" s="41"/>
       <c r="M37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1559,15 +1563,13 @@
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
       <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
+      <c r="H38" s="20"/>
       <c r="I38" s="13">
-        <v>0.0625</v>
-      </c>
-      <c r="J38" s="26">
-        <v>0.041666666666666664</v>
-      </c>
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="J38" s="27"/>
       <c r="K38" s="17"/>
-      <c r="L38" s="39"/>
+      <c r="L38" s="41"/>
       <c r="M38" s="11">
         <f t="shared" si="1"/>
         <v>0.1041666667</v>
@@ -1585,13 +1587,13 @@
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
       <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="13">
+      <c r="H39" s="20">
         <v>0.10416666666666667</v>
       </c>
+      <c r="I39" s="20"/>
+      <c r="J39" s="13"/>
       <c r="K39" s="17"/>
-      <c r="L39" s="39"/>
+      <c r="L39" s="41"/>
       <c r="M39" s="11">
         <f t="shared" si="1"/>
         <v>0.1041666667</v>
@@ -1611,7 +1613,7 @@
       <c r="I40" s="17"/>
       <c r="J40" s="17"/>
       <c r="K40" s="17"/>
-      <c r="L40" s="39"/>
+      <c r="L40" s="41"/>
       <c r="M40" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1635,7 +1637,7 @@
         <v>0.08333333333333333</v>
       </c>
       <c r="K41" s="20"/>
-      <c r="L41" s="39"/>
+      <c r="L41" s="41"/>
       <c r="M41" s="11">
         <f t="shared" si="1"/>
         <v>0.08333333333</v>
@@ -1657,9 +1659,11 @@
       <c r="I42" s="17"/>
       <c r="J42" s="17"/>
       <c r="K42" s="19">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="L42" s="48"/>
+        <v>0.125</v>
+      </c>
+      <c r="L42" s="49">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="M42" s="11">
         <f t="shared" si="1"/>
         <v>0.2083333333</v>
@@ -1679,7 +1683,7 @@
       <c r="I43" s="17"/>
       <c r="J43" s="17"/>
       <c r="K43" s="17"/>
-      <c r="L43" s="39"/>
+      <c r="L43" s="41"/>
       <c r="M43" s="11"/>
     </row>
     <row r="44">
@@ -1696,7 +1700,7 @@
         <v>0.020833333333333332</v>
       </c>
       <c r="G44" s="7">
-        <v>0.020833333333333332</v>
+        <v>0.0625</v>
       </c>
       <c r="H44" s="7">
         <v>0.020833333333333332</v>
@@ -1704,15 +1708,13 @@
       <c r="I44" s="7">
         <v>0.020833333333333332</v>
       </c>
-      <c r="J44" s="26">
+      <c r="J44" s="27">
         <v>0.041666666666666664</v>
       </c>
-      <c r="K44" s="26">
+      <c r="K44" s="27">
         <v>0.041666666666666664</v>
       </c>
-      <c r="L44" s="26">
-        <v>0.041666666666666664</v>
-      </c>
+      <c r="L44" s="50"/>
       <c r="M44" s="11">
         <f t="shared" ref="M44:M47" si="2">SUM(C44:L44)</f>
         <v>0.2083333333</v>
@@ -1736,7 +1738,7 @@
       <c r="K45" s="13">
         <v>0.0625</v>
       </c>
-      <c r="L45" s="49">
+      <c r="L45" s="51">
         <v>0.14583333333333334</v>
       </c>
       <c r="M45" s="11">
@@ -1760,7 +1762,7 @@
       <c r="I46" s="17"/>
       <c r="J46" s="17"/>
       <c r="K46" s="17"/>
-      <c r="L46" s="48">
+      <c r="L46" s="49">
         <v>0.08333333333333333</v>
       </c>
       <c r="M46" s="11">
@@ -1780,7 +1782,7 @@
       <c r="I47" s="17"/>
       <c r="J47" s="17"/>
       <c r="K47" s="17"/>
-      <c r="L47" s="39"/>
+      <c r="L47" s="41"/>
       <c r="M47" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1798,7 +1800,7 @@
       <c r="I48" s="17"/>
       <c r="J48" s="17"/>
       <c r="K48" s="17"/>
-      <c r="L48" s="39"/>
+      <c r="L48" s="41"/>
       <c r="M48" s="11"/>
     </row>
     <row r="49">
@@ -1815,7 +1817,7 @@
       <c r="I49" s="17"/>
       <c r="J49" s="17"/>
       <c r="K49" s="17"/>
-      <c r="L49" s="39"/>
+      <c r="L49" s="41"/>
       <c r="M49" s="11"/>
     </row>
     <row r="50">
@@ -1826,34 +1828,34 @@
         <v>0.75</v>
       </c>
       <c r="C50" s="7">
-        <v>0.020833333333333332</v>
+        <v>0.0625</v>
       </c>
       <c r="D50" s="13">
         <v>0.0625</v>
       </c>
-      <c r="E50" s="28">
-        <v>0.0625</v>
+      <c r="E50" s="23">
+        <v>0.10416666666666667</v>
       </c>
       <c r="F50" s="13">
         <v>0.0625</v>
       </c>
       <c r="G50" s="13">
-        <v>0.0625</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="H50" s="13">
-        <v>0.0625</v>
+        <v>0.020833333333333332</v>
       </c>
       <c r="I50" s="13">
         <v>0.10416666666666667</v>
       </c>
-      <c r="J50" s="13">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="K50" s="29">
-        <v>0.08333333333333333</v>
-      </c>
-      <c r="L50" s="49">
-        <v>0.125</v>
+      <c r="J50" s="23">
+        <v>0.0625</v>
+      </c>
+      <c r="K50" s="19">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="L50" s="51">
+        <v>0.08333333333333333</v>
       </c>
       <c r="M50" s="11">
         <f t="shared" ref="M50:M52" si="3">SUM(C50:L50)</f>
@@ -1878,90 +1880,90 @@
       <c r="I51" s="17"/>
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
-      <c r="L51" s="39"/>
+      <c r="L51" s="41"/>
       <c r="M51" s="11">
         <f t="shared" si="3"/>
         <v>0.125</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="50"/>
-      <c r="B52" s="40"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="40"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="40"/>
-      <c r="G52" s="50"/>
-      <c r="H52" s="40"/>
-      <c r="I52" s="50"/>
-      <c r="J52" s="40"/>
-      <c r="K52" s="51"/>
-      <c r="L52" s="40"/>
+      <c r="A52" s="52"/>
+      <c r="B52" s="43"/>
+      <c r="C52" s="52"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="52"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="52"/>
+      <c r="H52" s="43"/>
+      <c r="I52" s="52"/>
+      <c r="J52" s="43"/>
+      <c r="K52" s="53"/>
+      <c r="L52" s="43"/>
       <c r="M52" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="52"/>
+      <c r="A53" s="54"/>
       <c r="B53" s="11">
         <f t="shared" ref="B53:L53" si="4">SUM(B2:B52)</f>
         <v>3.666666667</v>
       </c>
       <c r="C53" s="11">
         <f t="shared" si="4"/>
-        <v>0.4166666667</v>
+        <v>0.3333333333</v>
       </c>
       <c r="D53" s="11">
         <f t="shared" si="4"/>
-        <v>0.3541666667</v>
+        <v>0.3958333333</v>
       </c>
       <c r="E53" s="11">
         <f t="shared" si="4"/>
-        <v>0.3125</v>
+        <v>0.3958333333</v>
       </c>
       <c r="F53" s="11">
         <f t="shared" si="4"/>
-        <v>0.3541666667</v>
+        <v>0.3333333333</v>
       </c>
       <c r="G53" s="11">
         <f t="shared" si="4"/>
-        <v>0.3333333333</v>
+        <v>0.3541666667</v>
       </c>
       <c r="H53" s="11">
         <f t="shared" si="4"/>
-        <v>0.375</v>
+        <v>0.3958333333</v>
       </c>
       <c r="I53" s="11">
         <f t="shared" si="4"/>
-        <v>0.3541666667</v>
+        <v>0.3958333333</v>
       </c>
       <c r="J53" s="11">
         <f t="shared" si="4"/>
-        <v>0.375</v>
+        <v>0.3541666667</v>
       </c>
       <c r="K53" s="11">
         <f t="shared" si="4"/>
-        <v>0.3958333333</v>
+        <v>0.3125</v>
       </c>
       <c r="L53" s="11">
         <f t="shared" si="4"/>
         <v>0.3958333333</v>
       </c>
-      <c r="M53" s="52"/>
+      <c r="M53" s="54"/>
     </row>
     <row r="54">
-      <c r="A54" s="52"/>
-      <c r="B54" s="52"/>
-      <c r="C54" s="52"/>
-      <c r="D54" s="52"/>
-      <c r="E54" s="52"/>
-      <c r="F54" s="52"/>
-      <c r="G54" s="52"/>
-      <c r="H54" s="52"/>
-      <c r="I54" s="52"/>
-      <c r="J54" s="52"/>
-      <c r="K54" s="52"/>
+      <c r="A54" s="54"/>
+      <c r="B54" s="54"/>
+      <c r="C54" s="54"/>
+      <c r="D54" s="54"/>
+      <c r="E54" s="54"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="54"/>
+      <c r="H54" s="54"/>
+      <c r="I54" s="54"/>
+      <c r="J54" s="54"/>
+      <c r="K54" s="54"/>
       <c r="L54" s="11">
         <f>SUM(C53:L53)</f>
         <v>3.666666667</v>

</xml_diff>